<commit_message>
Loader fix and excel update
</commit_message>
<xml_diff>
--- a/public/Bulk Map.xlsx
+++ b/public/Bulk Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U1072231\Desktop\PD\UI\pd-ui\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8AC669-3898-4908-BFBE-363F445EF72C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DB1698-3BA7-4D79-949A-5CD42DE1CF42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>protocol</t>
   </si>
@@ -42,13 +42,10 @@
     <t>userRole</t>
   </si>
   <si>
-    <t>Note:</t>
-  </si>
-  <si>
-    <t>Valid Values for Follow is "1" or "0"(1 Means Yes and 0 Means No)</t>
-  </si>
-  <si>
-    <t>Add only numbers in UserID field(Example : Add 123456 if your ID is Q123456/U123456)</t>
+    <t>Note:
+Add only numbers in UserID field(Example : Add 123456 if your ID is Q123456/U123456)
+Valid Values for Follow is "1" or "0"(1 Means Yes and 0 Means No)
+Valid Values for userRole is "primary" or "secondary"</t>
   </si>
 </sst>
 </file>
@@ -64,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,12 +71,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,10 +87,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,20 +375,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.54296875" customWidth="1"/>
     <col min="8" max="8" width="74.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -409,19 +405,23 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H3" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>